<commit_message>
Finalizing Pattern begin adding labels
</commit_message>
<xml_diff>
--- a/Original Plot Work/1917 Victory Map/Victory Map of 1917 State Types.xlsx
+++ b/Original Plot Work/1917 Victory Map/Victory Map of 1917 State Types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RBY11\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A7BA31-42AD-4016-9B3A-62D1CAF93324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C62CDF-327E-4ABB-AD67-7F354F553CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="2400" windowWidth="21600" windowHeight="11835" xr2:uid="{DA0E77D7-1B92-4340-9A8D-E4AF89B9DC01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DA0E77D7-1B92-4340-9A8D-E4AF89B9DC01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
   <si>
     <t>State</t>
   </si>
@@ -332,15 +332,6 @@
   </si>
   <si>
     <t>Connecticut</t>
-  </si>
-  <si>
-    <t>circle</t>
-  </si>
-  <si>
-    <t>stripe</t>
-  </si>
-  <si>
-    <t>none</t>
   </si>
   <si>
     <t>test</t>
@@ -718,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC3D07F-35FF-460F-9A33-7A00C188A41D}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +726,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,13 +734,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
-        <v>99</v>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -757,13 +748,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
       </c>
-      <c r="D3" t="s">
-        <v>99</v>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,13 +762,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>53</v>
       </c>
-      <c r="D4" t="s">
-        <v>99</v>
+      <c r="D4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,13 +776,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>
       </c>
-      <c r="D5" t="s">
-        <v>99</v>
+      <c r="D5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -799,13 +790,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
         <v>55</v>
       </c>
-      <c r="D6" t="s">
-        <v>99</v>
+      <c r="D6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -813,13 +804,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
       </c>
-      <c r="D7" t="s">
-        <v>99</v>
+      <c r="D7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -827,13 +818,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
         <v>57</v>
       </c>
-      <c r="D8" t="s">
-        <v>99</v>
+      <c r="D8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -841,13 +832,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
         <v>58</v>
       </c>
-      <c r="D9" t="s">
-        <v>99</v>
+      <c r="D9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -855,13 +846,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
         <v>59</v>
       </c>
-      <c r="D10" t="s">
-        <v>99</v>
+      <c r="D10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -869,13 +860,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
         <v>60</v>
       </c>
-      <c r="D11" t="s">
-        <v>99</v>
+      <c r="D11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -883,13 +874,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
         <v>61</v>
       </c>
-      <c r="D12" t="s">
-        <v>99</v>
+      <c r="D12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,13 +888,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" t="s">
-        <v>99</v>
+      <c r="D13">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,13 +902,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
         <v>63</v>
       </c>
-      <c r="D14" t="s">
-        <v>99</v>
+      <c r="D14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -925,13 +916,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
         <v>64</v>
       </c>
-      <c r="D15" t="s">
-        <v>100</v>
+      <c r="D15">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -939,13 +930,13 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
         <v>65</v>
       </c>
-      <c r="D16" t="s">
-        <v>100</v>
+      <c r="D16">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -953,13 +944,13 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
         <v>97</v>
       </c>
-      <c r="D17" t="s">
-        <v>100</v>
+      <c r="D17">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -967,13 +958,13 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
         <v>66</v>
       </c>
-      <c r="D18" t="s">
-        <v>100</v>
+      <c r="D18">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -981,13 +972,13 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
         <v>67</v>
       </c>
-      <c r="D19" t="s">
-        <v>100</v>
+      <c r="D19">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -995,13 +986,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
         <v>68</v>
       </c>
-      <c r="D20" t="s">
-        <v>100</v>
+      <c r="D20">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1009,13 +1000,13 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
         <v>69</v>
       </c>
-      <c r="D21" t="s">
-        <v>100</v>
+      <c r="D21">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,13 +1014,13 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
         <v>70</v>
       </c>
-      <c r="D22" t="s">
-        <v>100</v>
+      <c r="D22">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,13 +1028,13 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
         <v>71</v>
       </c>
-      <c r="D23" t="s">
-        <v>100</v>
+      <c r="D23">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1051,13 +1042,13 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
         <v>72</v>
       </c>
-      <c r="D24" t="s">
-        <v>100</v>
+      <c r="D24">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1065,13 +1056,13 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
         <v>98</v>
       </c>
-      <c r="D25" t="s">
-        <v>100</v>
+      <c r="D25">
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1079,13 +1070,13 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
         <v>73</v>
       </c>
-      <c r="D26" t="s">
-        <v>100</v>
+      <c r="D26">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1093,13 +1084,13 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
         <v>74</v>
       </c>
-      <c r="D27" t="s">
-        <v>100</v>
+      <c r="D27">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1107,13 +1098,13 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
         <v>75</v>
       </c>
-      <c r="D28" t="s">
-        <v>100</v>
+      <c r="D28">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1121,13 +1112,13 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
         <v>76</v>
       </c>
-      <c r="D29" t="s">
-        <v>99</v>
+      <c r="D29">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1135,13 +1126,13 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
         <v>77</v>
       </c>
-      <c r="D30" t="s">
-        <v>99</v>
+      <c r="D30">
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,13 +1140,13 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
         <v>78</v>
       </c>
-      <c r="D31" t="s">
-        <v>99</v>
+      <c r="D31">
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1163,13 +1154,13 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
         <v>79</v>
       </c>
-      <c r="D32" t="s">
-        <v>100</v>
+      <c r="D32">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1177,13 +1168,13 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
         <v>80</v>
       </c>
-      <c r="D33" t="s">
-        <v>100</v>
+      <c r="D33">
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1191,13 +1182,13 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
         <v>81</v>
       </c>
-      <c r="D34" t="s">
-        <v>99</v>
+      <c r="D34">
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1205,13 +1196,13 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
         <v>82</v>
       </c>
-      <c r="D35" t="s">
-        <v>99</v>
+      <c r="D35">
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,13 +1210,13 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
         <v>83</v>
       </c>
-      <c r="D36" t="s">
-        <v>101</v>
+      <c r="D36">
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1233,13 +1224,13 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C37" t="s">
         <v>84</v>
       </c>
-      <c r="D37" t="s">
-        <v>101</v>
+      <c r="D37">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1247,13 +1238,13 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
         <v>85</v>
       </c>
-      <c r="D38" t="s">
-        <v>101</v>
+      <c r="D38">
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1261,13 +1252,13 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C39" t="s">
         <v>86</v>
       </c>
-      <c r="D39" t="s">
-        <v>101</v>
+      <c r="D39">
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1275,13 +1266,13 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
         <v>87</v>
       </c>
-      <c r="D40" t="s">
-        <v>101</v>
+      <c r="D40">
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1289,13 +1280,13 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C41" t="s">
         <v>88</v>
       </c>
-      <c r="D41" t="s">
-        <v>101</v>
+      <c r="D41">
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1303,13 +1294,13 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
         <v>89</v>
       </c>
-      <c r="D42" t="s">
-        <v>101</v>
+      <c r="D42">
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1317,13 +1308,13 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C43" t="s">
         <v>90</v>
       </c>
-      <c r="D43" t="s">
-        <v>101</v>
+      <c r="D43">
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1331,13 +1322,13 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
         <v>91</v>
       </c>
-      <c r="D44" t="s">
-        <v>101</v>
+      <c r="D44">
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1345,13 +1336,13 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C45" t="s">
         <v>92</v>
       </c>
-      <c r="D45" t="s">
-        <v>101</v>
+      <c r="D45">
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1359,13 +1350,13 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
         <v>93</v>
       </c>
-      <c r="D46" t="s">
-        <v>101</v>
+      <c r="D46">
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1373,13 +1364,13 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s">
         <v>94</v>
       </c>
-      <c r="D47" t="s">
-        <v>101</v>
+      <c r="D47">
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1387,13 +1378,13 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
         <v>95</v>
       </c>
-      <c r="D48" t="s">
-        <v>101</v>
+      <c r="D48">
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1401,13 +1392,13 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
         <v>96</v>
       </c>
-      <c r="D49" t="s">
-        <v>99</v>
+      <c r="D49">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>